<commit_message>
add images for logos, create skeleton for views
</commit_message>
<xml_diff>
--- a/docs/qualites.xlsx
+++ b/docs/qualites.xlsx
@@ -157,10 +157,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Mass &amp; Stacks</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>HAVEN</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -258,6 +254,10 @@
   </si>
   <si>
     <t>sporty</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maas &amp; Stacks</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -641,8 +641,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85:A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -667,10 +667,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
         <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -678,10 +678,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -689,10 +689,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -700,10 +700,10 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -711,10 +711,10 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -722,10 +722,10 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -733,10 +733,10 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -744,10 +744,10 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -755,10 +755,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -766,10 +766,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -777,10 +777,10 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -788,10 +788,10 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -799,10 +799,10 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -810,10 +810,10 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -821,10 +821,10 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -832,10 +832,10 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -843,10 +843,10 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -854,10 +854,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -865,10 +865,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -876,10 +876,10 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -887,10 +887,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -898,10 +898,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -909,10 +909,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -920,10 +920,10 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -931,10 +931,10 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -942,10 +942,10 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
         <v>56</v>
-      </c>
-      <c r="C27" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -953,10 +953,10 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -964,10 +964,10 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -975,10 +975,10 @@
         <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -986,7 +986,7 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
@@ -997,7 +997,7 @@
         <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
@@ -1008,10 +1008,10 @@
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1019,10 +1019,10 @@
         <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1030,7 +1030,7 @@
         <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -1041,10 +1041,10 @@
         <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1052,10 +1052,10 @@
         <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1063,10 +1063,10 @@
         <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1074,7 +1074,7 @@
         <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
@@ -1085,10 +1085,10 @@
         <v>25</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1096,7 +1096,7 @@
         <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
@@ -1107,10 +1107,10 @@
         <v>25</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1118,7 +1118,7 @@
         <v>25</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
         <v>3</v>
@@ -1129,7 +1129,7 @@
         <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C44" t="s">
         <v>3</v>
@@ -1140,10 +1140,10 @@
         <v>26</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1151,10 +1151,10 @@
         <v>26</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1162,7 +1162,7 @@
         <v>26</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C47" t="s">
         <v>3</v>
@@ -1173,10 +1173,10 @@
         <v>26</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1184,7 +1184,7 @@
         <v>26</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" t="s">
         <v>0</v>
@@ -1195,10 +1195,10 @@
         <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1206,10 +1206,10 @@
         <v>27</v>
       </c>
       <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" t="s">
         <v>56</v>
-      </c>
-      <c r="C51" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1217,10 +1217,10 @@
         <v>27</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1228,10 +1228,10 @@
         <v>27</v>
       </c>
       <c r="B53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1239,10 +1239,10 @@
         <v>27</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1250,10 +1250,10 @@
         <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1261,10 +1261,10 @@
         <v>28</v>
       </c>
       <c r="B56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1272,10 +1272,10 @@
         <v>28</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1283,10 +1283,10 @@
         <v>28</v>
       </c>
       <c r="B58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1294,7 +1294,7 @@
         <v>28</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
@@ -1305,7 +1305,7 @@
         <v>28</v>
       </c>
       <c r="B60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C60" t="s">
         <v>3</v>
@@ -1316,7 +1316,7 @@
         <v>29</v>
       </c>
       <c r="B61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
@@ -1327,10 +1327,10 @@
         <v>29</v>
       </c>
       <c r="B62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1338,7 +1338,7 @@
         <v>29</v>
       </c>
       <c r="B63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C63" t="s">
         <v>8</v>
@@ -1349,7 +1349,7 @@
         <v>29</v>
       </c>
       <c r="B64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C64" t="s">
         <v>7</v>
@@ -1360,7 +1360,7 @@
         <v>29</v>
       </c>
       <c r="B65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
@@ -1371,7 +1371,7 @@
         <v>29</v>
       </c>
       <c r="B66" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C66" t="s">
         <v>9</v>
@@ -1382,10 +1382,10 @@
         <v>30</v>
       </c>
       <c r="B67" t="s">
+        <v>55</v>
+      </c>
+      <c r="C67" t="s">
         <v>56</v>
-      </c>
-      <c r="C67" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1393,10 +1393,10 @@
         <v>30</v>
       </c>
       <c r="B68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C68" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1404,7 +1404,7 @@
         <v>30</v>
       </c>
       <c r="B69" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C69" t="s">
         <v>10</v>
@@ -1415,10 +1415,10 @@
         <v>30</v>
       </c>
       <c r="B70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1426,10 +1426,10 @@
         <v>30</v>
       </c>
       <c r="B71" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C71" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1437,7 +1437,7 @@
         <v>30</v>
       </c>
       <c r="B72" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C72" t="s">
         <v>0</v>
@@ -1448,7 +1448,7 @@
         <v>31</v>
       </c>
       <c r="B73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C73" t="s">
         <v>6</v>
@@ -1459,10 +1459,10 @@
         <v>31</v>
       </c>
       <c r="B74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C74" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1470,10 +1470,10 @@
         <v>31</v>
       </c>
       <c r="B75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C75" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1481,7 +1481,7 @@
         <v>31</v>
       </c>
       <c r="B76" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
@@ -1492,7 +1492,7 @@
         <v>31</v>
       </c>
       <c r="B77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C77" t="s">
         <v>5</v>
@@ -1503,7 +1503,7 @@
         <v>31</v>
       </c>
       <c r="B78" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C78" t="s">
         <v>9</v>
@@ -1514,7 +1514,7 @@
         <v>32</v>
       </c>
       <c r="B79" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C79" t="s">
         <v>9</v>
@@ -1525,7 +1525,7 @@
         <v>32</v>
       </c>
       <c r="B80" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C80" t="s">
         <v>5</v>
@@ -1536,10 +1536,10 @@
         <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C81" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1547,7 +1547,7 @@
         <v>33</v>
       </c>
       <c r="B82" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C82" t="s">
         <v>2</v>
@@ -1558,10 +1558,10 @@
         <v>33</v>
       </c>
       <c r="B83" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C83" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1569,73 +1569,73 @@
         <v>33</v>
       </c>
       <c r="B84" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C84" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B85" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C85" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B86" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C86" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B87" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C87" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B88" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C88" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B89" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C89" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B90" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C90" t="s">
         <v>3</v>
@@ -1643,10 +1643,10 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B91" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C91" t="s">
         <v>5</v>
@@ -1654,32 +1654,32 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B92" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C92" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B93" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C93" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B94" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C94" t="s">
         <v>3</v>
@@ -1687,54 +1687,54 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B95" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C95" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B96" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C96" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B97" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C97" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B98" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C98" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B99" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C99" t="s">
         <v>6</v>
@@ -1742,10 +1742,10 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B100" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C100" t="s">
         <v>11</v>
@@ -1753,21 +1753,21 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B101" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C101" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B102" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C102" t="s">
         <v>0</v>

</xml_diff>